<commit_message>
update code with drop Na values
</commit_message>
<xml_diff>
--- a/processed/SCHCT_24.03.2025_vendor_list_SBI_Gorhe.xlsx
+++ b/processed/SCHCT_24.03.2025_vendor_list_SBI_Gorhe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,10 +497,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4240035697</v>
+        <v>4240035910</v>
       </c>
       <c r="B2" t="n">
-        <v>36428</v>
+        <v>11800</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -514,28 +514,28 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Vikram Kisan Seva Kendra</t>
+          <t>Sri Tulsi Trust- Tulsi Books</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>60075347347</t>
+          <t>910010014548454</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>MAHB0000429</t>
+          <t>UTIB0001004</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Vikramgad</t>
+          <t>Chowpatty</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Vikramgad</t>
+          <t>Chowpatty</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -545,16 +545,16 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>O|A|Vikram Kisan Seva Kendra|60075347347||MAHB0000429|Vikramgad|Vikramgad|India</t>
+          <t>O|A|Sri Tulsi Trust- Tulsi Books|910010014548454||UTIB0001004|Chowpatty|Chowpatty|India</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4240034900</v>
+        <v>4240035907</v>
       </c>
       <c r="B3" t="n">
-        <v>30000</v>
+        <v>10209</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -568,28 +568,28 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ganesh Ashok Sarode</t>
+          <t>TATA AIG GENERAL INSURANCE CO</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>50100286551314</t>
+          <t>0005922018</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>HDFC0002865</t>
+          <t>DEUT0784BBY</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Jawhar</t>
+          <t>Mumbai</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Jawhar</t>
+          <t>Mumbai</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -599,16 +599,16 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>O|A|Ganesh Ashok Sarode|50100286551314||HDFC0002865|Jawhar|Jawhar|India</t>
+          <t>O|A|TATA AIG GENERAL INSURANCE CO|0005922018||DEUT0784BBY|Mumbai|Mumbai|India</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4240034888</v>
+        <v>4240035886</v>
       </c>
       <c r="B4" t="n">
-        <v>376937</v>
+        <v>1805</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -622,28 +622,28 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Prathmesh Aniruddha Patil</t>
+          <t>Mukund Dhanawade</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>50200051636399</t>
+          <t>695010085299</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>HDFC0002246</t>
+          <t>KKBK0000638</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Wada</t>
+          <t>Mumbai Lower Parel</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Wada</t>
+          <t>Mumbai Lower Parel</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -653,16 +653,16 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>O|A|Prathmesh Aniruddha Patil|50200051636399||HDFC0002246|Wada|Wada|India</t>
+          <t>O|A|Mukund Dhanawade|695010085299||KKBK0000638|Mumbai Lower Parel|Mumbai Lower Parel|India</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4240034881</v>
+        <v>4240035815</v>
       </c>
       <c r="B5" t="n">
-        <v>20000</v>
+        <v>2247</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -676,28 +676,28 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Shivkumar Rajbhar</t>
+          <t>Shekhar Laxman Chavan</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>453002120006111</t>
+          <t>41678100000806</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>UBIN0545309</t>
+          <t>BARB0WATHAR</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Sadat Raiway</t>
+          <t xml:space="preserve">Wathar </t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Sadat Raiway</t>
+          <t xml:space="preserve">Wathar </t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -707,20 +707,20 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>O|A|Shivkumar Rajbhar|453002120006111||UBIN0545309|Sadat Raiway|Sadat Raiway|India</t>
+          <t>O|A|Shekhar Laxman Chavan|41678100000806||BARB0WATHAR|Wathar |Wathar |India</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4240034879</v>
+        <v>4240035814</v>
       </c>
       <c r="B6" t="n">
-        <v>20300</v>
+        <v>955</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>O</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -730,28 +730,28 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Pandhari Bapu Dhadaga</t>
+          <t>Vaibhav Chavan</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>33319830459</t>
+          <t>41678100000494</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>SBIN0000444</t>
+          <t>BARB0WATHAR</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Palghar</t>
+          <t xml:space="preserve">Wathar </t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Palghar</t>
+          <t xml:space="preserve">Wathar </t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -761,20 +761,20 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>S|A|Pandhari Bapu Dhadaga|33319830459||SBIN0000444|Palghar|Palghar|India</t>
+          <t>O|A|Vaibhav Chavan|41678100000494||BARB0WATHAR|Wathar |Wathar |India</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4240034867</v>
+        <v>4240035810</v>
       </c>
       <c r="B7" t="n">
-        <v>15000</v>
+        <v>16500</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>O</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -784,28 +784,28 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Vinay Atmaram Junghare</t>
+          <t>Ranjana  Ravindra Bhoir</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>42084482381</t>
+          <t>55605007149</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>SBIN0000473</t>
+          <t>MAHG0005605</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Satara</t>
+          <t>Alonde</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Satara</t>
+          <t>Alonde</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -815,20 +815,20 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>S|A|Vinay Atmaram Junghare|42084482381||SBIN0000473|Satara|Satara|India</t>
+          <t>O|A|Ranjana  Ravindra Bhoir|55605007149||MAHG0005605|Alonde|Alonde|India</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>4240034866</v>
+        <v>4240035803</v>
       </c>
       <c r="B8" t="n">
-        <v>10000</v>
+        <v>248</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>O</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -838,28 +838,28 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Simantini Tejas khilare</t>
+          <t>Hemant Kondu Patil</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>40140257163</t>
+          <t>009210100011231</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>SBIN0007773</t>
+          <t>BKID0000092</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Gorhe</t>
+          <t>Boiser</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Gorhe</t>
+          <t>Boiser</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -869,16 +869,16 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>S|A|Simantini Tejas khilare|40140257163||SBIN0007773|Gorhe|Gorhe|India</t>
+          <t>O|A|Hemant Kondu Patil|009210100011231||BKID0000092|Boiser|Boiser|India</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4240034864</v>
+        <v>4240035799</v>
       </c>
       <c r="B9" t="n">
-        <v>22500</v>
+        <v>6435</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -892,28 +892,28 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Mukund Bhikaji Dhanawade</t>
+          <t>Laxman Sudhakar Padwale</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>695010085299</t>
+          <t>033910330510</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>KKBK0000638</t>
+          <t>IPOS0000001</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Lower Parel</t>
+          <t>Corporate Office</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Lower Parel</t>
+          <t>Corporate Office</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -923,20 +923,20 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>O|A|Mukund Bhikaji Dhanawade|695010085299||KKBK0000638| Lower Parel| Lower Parel|India</t>
+          <t>O|A|Laxman Sudhakar Padwale|033910330510||IPOS0000001|Corporate Office|Corporate Office|India</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4240033805</v>
+        <v>4240035796</v>
       </c>
       <c r="B10" t="n">
-        <v>1395</v>
+        <v>198305</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>O</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -946,28 +946,28 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Bharat Xerox And Stationary</t>
+          <t>Bhagirath Electricals &amp; Borewell</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>38166911649</t>
+          <t>60056433432</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>SBIN0001050</t>
+          <t>MAHB0000429</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jawhar </t>
+          <t>Vikramgad</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jawhar </t>
+          <t>Vikramgad</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -977,16 +977,16 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>S|A|Bharat Xerox And Stationary|38166911649||SBIN0001050|Jawhar |Jawhar |India</t>
+          <t>O|A|Bhagirath Electricals &amp; Borewell|60056433432||MAHB0000429|Vikramgad|Vikramgad|India</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4240033509</v>
+        <v>4240035785</v>
       </c>
       <c r="B11" t="n">
-        <v>1200</v>
+        <v>85374</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1000,28 +1000,28 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Rohidas Hemant Hadal</t>
+          <t>Kore Mining &amp; Crushing Pvt Ltd</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>50100126004764</t>
+          <t>396100100001108</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>HDFC0000733</t>
+          <t>SRCB0000396</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Bhiwandi</t>
+          <t>Boisar</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Bhiwandi</t>
+          <t>Boisar</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1031,29 +1031,515 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>O|A|Rohidas Hemant Hadal|50100126004764||HDFC0000733|Bhiwandi|Bhiwandi|India</t>
+          <t>O|A|Kore Mining &amp; Crushing Pvt Ltd|396100100001108||SRCB0000396|Boisar|Boisar|India</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="n">
+        <v>4240035782</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1533</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Ganesh Ashok Sarode</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>50100286551314</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>HDFC0002865</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Jawhar</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Jawhar</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>O|A|Ganesh Ashok Sarode|50100286551314||HDFC0002865|Jawhar|Jawhar|India</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>4240035773</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20945</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Vijay Hardware Stores</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>50200098814777</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>HDFC0007179</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Manor</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Manor</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>O|A|Vijay Hardware Stores|50200098814777||HDFC0007179|Manor|Manor|India</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4240035770</v>
+      </c>
+      <c r="B14" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Mohit Kumar</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>38796858574</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>SBIN0001143</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>SAUGOR UNIVERSITY</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>SAUGOR UNIVERSITY</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>S|A|Mohit Kumar|38796858574||SBIN0001143|SAUGOR UNIVERSITY|SAUGOR UNIVERSITY|India</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>4240035740</v>
+      </c>
+      <c r="B15" t="n">
+        <v>4036</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Ravi Shankar Lahange</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>35187115601</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>SBIN0007773</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Gorhe</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Gorhe</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>S|A|Ravi Shankar Lahange|35187115601||SBIN0007773|Gorhe|Gorhe|India</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>4240035699</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1783</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Dipak Mahadu Gavit</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>33523530337</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>SBIN0001050</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>JAWHAR</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>JAWHAR</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>S|A|Dipak Mahadu Gavit|33523530337||SBIN0001050|JAWHAR|JAWHAR|India</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>4240035698</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3084</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Bharat Xerox And Stationary</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>38166911649</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>SBIN0001050</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jawhar </t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jawhar </t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>S|A|Bharat Xerox And Stationary|38166911649||SBIN0001050|Jawhar |Jawhar |India</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>4240035427</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3939</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Nilesh Vitthal Dhapshi</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>41568298765</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>SBIN0007773</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Gorhe</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Gorhe</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>S|A|Nilesh Vitthal Dhapshi|41568298765||SBIN0007773|Gorhe|Gorhe|India</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>4240034980</v>
+      </c>
+      <c r="B19" t="n">
+        <v>17198</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Madhavi Suryaji Desai</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>60258069880</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>MAHB0000195</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Palghar</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Palghar</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>O|A|Madhavi Suryaji Desai|60258069880||MAHB0000195|Palghar|Palghar|India</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>4240036101</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3589</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Ankush Yadav</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>681518110001008</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>BKID0006815</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Subhanikheda</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Subhanikheda</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>O|A|Ankush Yadav|681518110001008||BKID0006815|Subhanikheda|Subhanikheda|India</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>533760</v>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="B21" t="n">
+        <v>404985</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>